<commit_message>
Update 1.4.1: QoL for Invoice WriteOffs and bug fixes
</commit_message>
<xml_diff>
--- a/pkg/excels/templates/Invoice Input Report.xlsx
+++ b/pkg/excels/templates/Invoice Input Report.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mamad\OneDrive\Desktop\ТГЭМ\backend-v2\pkg\excels\report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mamad\OneDrive\Desktop\ТГЭМ\backend-v2\pkg\excels\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEBA7B96-A89E-4C3D-BEB1-521C5835D9D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1395DE7-D49C-4A78-A88C-3075CDBFADAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -58,8 +58,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -87,8 +95,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -372,7 +381,7 @@
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R16" sqref="R16"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -385,31 +394,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>